<commit_message>
More radical changes ... Currently working on DataTable within spreadsheet.py
</commit_message>
<xml_diff>
--- a/TESTDATA/testing/Noten/NOTEN_1/Noten_11.G_1.xlsx
+++ b/TESTDATA/testing/Noten/NOTEN_1/Noten_11.G_1.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
-  <si>
-    <t xml:space="preserve">#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
   <si>
     <t xml:space="preserve">Noten</t>
   </si>
@@ -106,7 +103,7 @@
     <t xml:space="preserve">Schüler(in)</t>
   </si>
   <si>
-    <t xml:space="preserve">Maßstab</t>
+    <t xml:space="preserve">Gruppen</t>
   </si>
   <si>
     <t xml:space="preserve">De</t>
@@ -226,7 +223,7 @@
     <t xml:space="preserve">Anna Amundsen</t>
   </si>
   <si>
-    <t xml:space="preserve">Gym</t>
+    <t xml:space="preserve">G</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -407,7 +404,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -478,6 +475,10 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -564,7 +565,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,16 +581,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -607,18 +606,18 @@
     </row>
     <row r="2" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -638,55 +637,55 @@
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="S3" s="7"/>
       <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -694,18 +693,18 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
@@ -716,13 +715,13 @@
     </row>
     <row r="5" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -744,13 +743,13 @@
     </row>
     <row r="6" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -773,130 +772,130 @@
     <row r="7" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="44.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="H8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="K8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="M8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="N8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="R8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="S8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="T8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="U8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="V8" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="V8" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="13"/>
       <c r="E9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="N9" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="O9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="P9" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="Q9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="R9" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="R9" s="16" t="s">
+      <c r="S9" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="T9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="16" t="s">
+      <c r="U9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="V9" s="16" t="s">
         <v>64</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -925,264 +924,264 @@
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="G11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="19"/>
+      <c r="I11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="18" t="s">
+      <c r="K11" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="P11" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="R11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="U11" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="V11" s="18" t="s">
-        <v>74</v>
+      <c r="Q11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="U11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="V11" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18" t="s">
+      <c r="L12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="P12" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="R12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="S12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="T12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="U12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="V12" s="18" t="s">
-        <v>74</v>
+      <c r="Q12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="V12" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="C13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="G13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="18" t="s">
+      <c r="K13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="P13" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="R13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="U13" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="V13" s="18" t="s">
-        <v>74</v>
+      <c r="Q13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="V13" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="P14" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="R14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="T14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="U14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="V14" s="18" t="s">
-        <v>74</v>
+      <c r="R14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="U14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="V14" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>